<commit_message>
Cleaned up plant-community diversity files.
Replaced blank cells with 0 (to indicate absence of a species)
Saved .xls(x) files as .txt
</commit_message>
<xml_diff>
--- a/kw_raw_Data_Field2014/MAHdiversity.xlsx
+++ b/kw_raw_Data_Field2014/MAHdiversity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,72 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
-    <t>m01</t>
-  </si>
-  <si>
-    <t>m02</t>
-  </si>
-  <si>
-    <t>m03</t>
-  </si>
-  <si>
-    <t>m04</t>
-  </si>
-  <si>
-    <t>m05</t>
-  </si>
-  <si>
-    <t>m06</t>
-  </si>
-  <si>
-    <t>m07</t>
-  </si>
-  <si>
-    <t>m08</t>
-  </si>
-  <si>
-    <t>m09</t>
-  </si>
-  <si>
-    <t>m10</t>
-  </si>
-  <si>
-    <t>m11</t>
-  </si>
-  <si>
-    <t>m12</t>
-  </si>
-  <si>
-    <t>m13</t>
-  </si>
-  <si>
-    <t>m14</t>
-  </si>
-  <si>
-    <t>m15</t>
-  </si>
-  <si>
-    <t>m16</t>
-  </si>
-  <si>
-    <t>j11</t>
-  </si>
-  <si>
-    <t>j12</t>
-  </si>
-  <si>
-    <t>j13</t>
-  </si>
-  <si>
-    <t>j14</t>
-  </si>
-  <si>
-    <t>j15</t>
-  </si>
-  <si>
-    <t>j16</t>
-  </si>
-  <si>
     <t>Dandelion</t>
   </si>
   <si>
@@ -160,6 +94,72 @@
   </si>
   <si>
     <t>Spruce</t>
+  </si>
+  <si>
+    <t>m.01</t>
+  </si>
+  <si>
+    <t>m.02</t>
+  </si>
+  <si>
+    <t>m.03</t>
+  </si>
+  <si>
+    <t>m.04</t>
+  </si>
+  <si>
+    <t>m.05</t>
+  </si>
+  <si>
+    <t>m.06</t>
+  </si>
+  <si>
+    <t>m.07</t>
+  </si>
+  <si>
+    <t>m.08</t>
+  </si>
+  <si>
+    <t>m.09</t>
+  </si>
+  <si>
+    <t>m.10</t>
+  </si>
+  <si>
+    <t>m.11</t>
+  </si>
+  <si>
+    <t>m.12</t>
+  </si>
+  <si>
+    <t>m.13</t>
+  </si>
+  <si>
+    <t>m.14</t>
+  </si>
+  <si>
+    <t>m.15</t>
+  </si>
+  <si>
+    <t>m.16</t>
+  </si>
+  <si>
+    <t>j.11</t>
+  </si>
+  <si>
+    <t>j.12</t>
+  </si>
+  <si>
+    <t>j.13</t>
+  </si>
+  <si>
+    <t>j.14</t>
+  </si>
+  <si>
+    <t>j.15</t>
+  </si>
+  <si>
+    <t>j.16</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -546,75 +546,75 @@
         <v>2014</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -969,7 +969,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B26">
         <v>0</v>

</xml_diff>